<commit_message>
update suivi de projet + index + styles.css avec la création de la section operation
</commit_message>
<xml_diff>
--- a/Suivi_du_projet_3.xlsx
+++ b/Suivi_du_projet_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fabien\Documents\Fomation_Web_Junior\Projet_3\Oh my food\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D5295A-8016-4A4C-A0A4-487822747B8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020129EB-6FC1-47F0-8ACB-EB744E6F8BBD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{9F752919-229D-4E4C-9826-FBF72DE5CBCD}"/>
   </bookViews>
@@ -415,13 +415,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>819150</xdr:colOff>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>809625</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>9526</xdr:rowOff>
     </xdr:to>
@@ -445,7 +445,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11096625" y="0"/>
+          <a:off x="11125200" y="0"/>
           <a:ext cx="6486525" cy="3543301"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1165,7 +1165,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
creation of green tick in 4 restaurants pages
</commit_message>
<xml_diff>
--- a/Suivi_du_projet_3.xlsx
+++ b/Suivi_du_projet_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fabien\Documents\Fomation_Web_Junior\Projet_3\Oh my food\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020129EB-6FC1-47F0-8ACB-EB744E6F8BBD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9453D775-27FC-459B-91F1-F1F6AF6B057E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{9F752919-229D-4E4C-9826-FBF72DE5CBCD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{9F752919-229D-4E4C-9826-FBF72DE5CBCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Accueuil" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
   <si>
     <t>À faire</t>
   </si>
@@ -137,28 +137,58 @@
     <t>Questions</t>
   </si>
   <si>
-    <t>J'ai eu ce message quand j'ai importer cette image</t>
-  </si>
-  <si>
-    <t>Est-ce que je dois garder ce fichier</t>
-  </si>
-  <si>
-    <t>quelle convention de nommage de commit git utiliser</t>
-  </si>
-  <si>
-    <t>Comment tu ordonnes tes propriétés d'élément en css</t>
-  </si>
-  <si>
-    <t>dimension placement</t>
-  </si>
-  <si>
-    <t>mise en forme</t>
-  </si>
-  <si>
-    <t>ordre aphabetique</t>
-  </si>
-  <si>
-    <t>j'ai voulu créer une mixin pour faire un bouton mais le fichier ne fonctionne pas en dehors du dossier mixin</t>
+    <t>insérer le titre</t>
+  </si>
+  <si>
+    <t>créer la card</t>
+  </si>
+  <si>
+    <t>insérer l'image</t>
+  </si>
+  <si>
+    <t>placer l'image</t>
+  </si>
+  <si>
+    <t>zone texte</t>
+  </si>
+  <si>
+    <t>créer bouton nouveau</t>
+  </si>
+  <si>
+    <t>placer le bouton nouveau</t>
+  </si>
+  <si>
+    <t>créer le cœur</t>
+  </si>
+  <si>
+    <t>placer le cœur</t>
+  </si>
+  <si>
+    <t>créer le titre</t>
+  </si>
+  <si>
+    <t>card en css</t>
+  </si>
+  <si>
+    <t>font awasome &lt;i class="fa-regular fa-heart"&gt;&lt;/i&gt; fonctionne</t>
+  </si>
+  <si>
+    <t>font awasome &lt;i class="fa-light fa-heart"&gt;&lt;/i &gt; ne fonctionne pas pourquoi?</t>
+  </si>
+  <si>
+    <t>créer le footer</t>
+  </si>
+  <si>
+    <t>régler la hauteur et le background</t>
+  </si>
+  <si>
+    <t>liste ul li</t>
+  </si>
+  <si>
+    <t>logo</t>
+  </si>
+  <si>
+    <t>icone plus texte</t>
   </si>
 </sst>
 </file>
@@ -322,140 +352,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1085850</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2306863-A0AC-4ECC-8F67-938AB47A44EB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect l="6251" t="79362" r="75052" b="11748"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4619625" y="0"/>
-          <a:ext cx="6410325" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC273925-C470-4F09-A2B9-DED818B389C1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:srcRect l="-29" t="60378" r="93445" b="19989"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4619625" y="942975"/>
-          <a:ext cx="2257425" cy="2019300"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>809625</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Image 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80E2CB3B-1027-421D-B0BC-9AAE9D3B19C0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:srcRect l="61952" t="49729" r="19128" b="15823"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11125200" y="0"/>
-          <a:ext cx="6486525" cy="3543301"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -755,17 +651,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94BD509D-E542-475C-B8E9-F231F4DE40FE}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46:D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7265625" customWidth="1"/>
-    <col min="3" max="3" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
@@ -1045,42 +941,306 @@
       <c r="B25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
+      <c r="F25" s="5"/>
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
-      <c r="B26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
+      <c r="F26" s="5"/>
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A27" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="C27" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+      <c r="F27" s="5"/>
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="C28" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="F28" s="5"/>
       <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="4"/>
+    </row>
+    <row r="36" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="4"/>
+    </row>
+    <row r="37" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="4"/>
+    </row>
+    <row r="38" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="4"/>
+    </row>
+    <row r="40" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="4"/>
+    </row>
+    <row r="41" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="4"/>
+    </row>
+    <row r="42" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="4"/>
+    </row>
+    <row r="43" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="4"/>
+    </row>
+    <row r="44" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="4"/>
+    </row>
+    <row r="45" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+    </row>
+    <row r="46" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="4"/>
+    </row>
+    <row r="47" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="4"/>
+    </row>
+    <row r="48" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="4"/>
+    </row>
+    <row r="49" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="4"/>
+    </row>
+    <row r="50" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="4"/>
+    </row>
+    <row r="51" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+    </row>
+    <row r="52" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1162,10 +1322,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BFD491-A0CC-48C4-8562-39394FECE3A9}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1175,81 +1335,62 @@
     <col min="4" max="4" width="11.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="42" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
     </row>
-    <row r="14" spans="1:5" ht="42" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" s="7"/>
+    </row>
+    <row r="15" spans="1:1" ht="54" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="7"/>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>